<commit_message>
Added new feature for schedule
</commit_message>
<xml_diff>
--- a/01-Excel/3/Activities/02-Ins_BasicCharting/Solved/BasicCharts.xlsx
+++ b/01-Excel/3/Activities/02-Ins_BasicCharting/Solved/BasicCharts.xlsx
@@ -1,32 +1,131 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\OneDrive\Documents\WorkAndSchool\TeachingAssistant\DataViz\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\3\Activities\02-Ins_BasicCharting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johntaylor/2021_2022_CWRU_BootCamp/cwru-cle-virt-data-pt-07-2021-u-c/01-Excel/3/Activities/02-Ins_BasicCharting/Solved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="F83C7F0B9C5BB36C676B768E03FEC89EF1BFA6B5" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{F5E47B7C-E461-45D1-AFA9-F37C2DE297AD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8F01D3-CB80-EE41-847E-0DB866DFB9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14610" windowHeight="14070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14540" yWindow="500" windowWidth="29640" windowHeight="19120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Favorite Ice Cream Flavors" sheetId="1" r:id="rId1"/>
     <sheet name="Ice Cream Sales" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.23" hidden="1">'Ice Cream Sales'!$A$2:$A$11</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'Ice Cream Sales'!$B$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'Ice Cream Sales'!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'Ice Cream Sales'!$C$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'Ice Cream Sales'!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'Ice Cream Sales'!$D$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'Ice Cream Sales'!$D$2:$D$11</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'Ice Cream Sales'!$E$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'Ice Cream Sales'!$E$2:$E$11</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'Ice Cream Sales'!$F$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'Ice Cream Sales'!$F$2:$F$11</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'Ice Cream Sales'!$G$1</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'Ice Cream Sales'!$G$2:$G$11</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'Ice Cream Sales'!$H$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'Ice Cream Sales'!$H$2:$H$11</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'Ice Cream Sales'!$I$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'Ice Cream Sales'!$I$2:$I$11</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'Ice Cream Sales'!$J$1</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'Ice Cream Sales'!$J$2:$J$11</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'Ice Cream Sales'!$K$1</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'Ice Cream Sales'!$K$2:$K$11</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'Ice Cream Sales'!$L$1</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">'Ice Cream Sales'!$L$2:$L$11</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">'Ice Cream Sales'!$A$10</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">'Ice Cream Sales'!$A$11</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">'Ice Cream Sales'!$A$2</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">'Ice Cream Sales'!$A$3</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">'Ice Cream Sales'!$A$4</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">'Ice Cream Sales'!$A$5</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">'Ice Cream Sales'!$A$6</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">'Ice Cream Sales'!$A$7</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">'Ice Cream Sales'!$A$8</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">'Ice Cream Sales'!$A$9</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">'Ice Cream Sales'!$B$10:$L$10</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">'Ice Cream Sales'!$B$11:$L$11</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">'Ice Cream Sales'!$B$1:$L$1</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">'Ice Cream Sales'!$B$2:$L$2</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">'Ice Cream Sales'!$B$3:$L$3</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">'Ice Cream Sales'!$B$4:$L$4</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">'Ice Cream Sales'!$B$5:$L$5</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">'Ice Cream Sales'!$B$6:$L$6</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">'Ice Cream Sales'!$B$7:$L$7</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">'Ice Cream Sales'!$B$8:$L$8</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">'Ice Cream Sales'!$B$9:$L$9</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'Ice Cream Sales'!$A$2:$A$11</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Ice Cream Sales'!$B$1</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">'Ice Cream Sales'!$F$2:$F$11</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">'Ice Cream Sales'!$G$1</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">'Ice Cream Sales'!$G$2:$G$11</definedName>
+    <definedName name="_xlchart.v2.13" hidden="1">'Ice Cream Sales'!$H$1</definedName>
+    <definedName name="_xlchart.v2.14" hidden="1">'Ice Cream Sales'!$H$2:$H$11</definedName>
+    <definedName name="_xlchart.v2.15" hidden="1">'Ice Cream Sales'!$I$1</definedName>
+    <definedName name="_xlchart.v2.16" hidden="1">'Ice Cream Sales'!$I$2:$I$11</definedName>
+    <definedName name="_xlchart.v2.17" hidden="1">'Ice Cream Sales'!$J$1</definedName>
+    <definedName name="_xlchart.v2.18" hidden="1">'Ice Cream Sales'!$J$2:$J$11</definedName>
+    <definedName name="_xlchart.v2.19" hidden="1">'Ice Cream Sales'!$K$1</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Ice Cream Sales'!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v2.20" hidden="1">'Ice Cream Sales'!$K$2:$K$11</definedName>
+    <definedName name="_xlchart.v2.21" hidden="1">'Ice Cream Sales'!$L$1</definedName>
+    <definedName name="_xlchart.v2.22" hidden="1">'Ice Cream Sales'!$L$2:$L$11</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Ice Cream Sales'!$C$1</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'Ice Cream Sales'!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">'Ice Cream Sales'!$D$1</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">'Ice Cream Sales'!$D$2:$D$11</definedName>
+    <definedName name="_xlchart.v2.67" hidden="1">'Ice Cream Sales'!$A$10</definedName>
+    <definedName name="_xlchart.v2.68" hidden="1">'Ice Cream Sales'!$A$11</definedName>
+    <definedName name="_xlchart.v2.69" hidden="1">'Ice Cream Sales'!$A$2</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">'Ice Cream Sales'!$E$1</definedName>
+    <definedName name="_xlchart.v2.70" hidden="1">'Ice Cream Sales'!$A$3</definedName>
+    <definedName name="_xlchart.v2.71" hidden="1">'Ice Cream Sales'!$A$4</definedName>
+    <definedName name="_xlchart.v2.72" hidden="1">'Ice Cream Sales'!$A$5</definedName>
+    <definedName name="_xlchart.v2.73" hidden="1">'Ice Cream Sales'!$A$6</definedName>
+    <definedName name="_xlchart.v2.74" hidden="1">'Ice Cream Sales'!$A$7</definedName>
+    <definedName name="_xlchart.v2.75" hidden="1">'Ice Cream Sales'!$A$8</definedName>
+    <definedName name="_xlchart.v2.76" hidden="1">'Ice Cream Sales'!$A$9</definedName>
+    <definedName name="_xlchart.v2.77" hidden="1">'Ice Cream Sales'!$B$10:$L$10</definedName>
+    <definedName name="_xlchart.v2.78" hidden="1">'Ice Cream Sales'!$B$11:$L$11</definedName>
+    <definedName name="_xlchart.v2.79" hidden="1">'Ice Cream Sales'!$B$1:$L$1</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">'Ice Cream Sales'!$E$2:$E$11</definedName>
+    <definedName name="_xlchart.v2.80" hidden="1">'Ice Cream Sales'!$B$2:$L$2</definedName>
+    <definedName name="_xlchart.v2.81" hidden="1">'Ice Cream Sales'!$B$3:$L$3</definedName>
+    <definedName name="_xlchart.v2.82" hidden="1">'Ice Cream Sales'!$B$4:$L$4</definedName>
+    <definedName name="_xlchart.v2.83" hidden="1">'Ice Cream Sales'!$B$5:$L$5</definedName>
+    <definedName name="_xlchart.v2.84" hidden="1">'Ice Cream Sales'!$B$6:$L$6</definedName>
+    <definedName name="_xlchart.v2.85" hidden="1">'Ice Cream Sales'!$B$7:$L$7</definedName>
+    <definedName name="_xlchart.v2.86" hidden="1">'Ice Cream Sales'!$B$8:$L$8</definedName>
+    <definedName name="_xlchart.v2.87" hidden="1">'Ice Cream Sales'!$B$9:$L$9</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">'Ice Cream Sales'!$F$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Vanilla</t>
   </si>
@@ -101,6 +200,9 @@
   </si>
   <si>
     <t>Dec</t>
+  </si>
+  <si>
+    <t>Line Graph?</t>
   </si>
 </sst>
 </file>
@@ -494,62 +596,8 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
+            <c:extLst/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1341,36 +1389,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1398,7 +1416,11 @@
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="50800" dir="5400000" sx="1000" sy="1000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000"/>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1880,7 +1902,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$6</c15:sqref>
@@ -1909,7 +1931,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -1956,7 +1978,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$6:$L$6</c15:sqref>
@@ -2003,7 +2025,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2016,7 +2038,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$7</c15:sqref>
@@ -2045,7 +2067,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2092,7 +2114,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$7:$L$7</c15:sqref>
@@ -2139,7 +2161,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2152,7 +2174,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$8</c15:sqref>
@@ -2183,7 +2205,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2230,7 +2252,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$8:$L$8</c15:sqref>
@@ -2277,7 +2299,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2290,7 +2312,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$9</c15:sqref>
@@ -2321,7 +2343,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2368,7 +2390,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$9:$L$9</c15:sqref>
@@ -2415,7 +2437,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2428,7 +2450,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$10</c15:sqref>
@@ -2459,7 +2481,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2506,7 +2528,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$10:$L$10</c15:sqref>
@@ -2553,7 +2575,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2566,7 +2588,7 @@
                 <c:order val="9"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$A$11</c15:sqref>
@@ -2597,7 +2619,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$1:$L$1</c15:sqref>
@@ -2644,7 +2666,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Ice Cream Sales'!$B$11:$L$11</c15:sqref>
@@ -2691,7 +2713,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-8B0B-41D6-BCCA-6C2E7079979C}"/>
                   </c:ext>
@@ -2732,9 +2754,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -4621,13 +4642,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
+      <xdr:colOff>828675</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>126205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>507206</xdr:colOff>
+      <xdr:colOff>469106</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>14288</xdr:rowOff>
     </xdr:to>
@@ -4954,18 +4975,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="20.73046875" customWidth="1"/>
+    <col min="1" max="8" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -4978,7 +4999,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4990,7 +5011,7 @@
         <v>0.11166666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5002,7 +5023,7 @@
         <v>8.8333333333333333E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5014,7 +5035,7 @@
         <v>0.10666666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5026,7 +5047,7 @@
         <v>0.15666666666666668</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5038,7 +5059,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5050,7 +5071,7 @@
         <v>0.13166666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5062,7 +5083,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5073,8 +5094,11 @@
         <f t="shared" si="0"/>
         <v>6.8333333333333329E-2</v>
       </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5086,7 +5110,7 @@
         <v>5.6666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5098,12 +5122,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <f>SUM(B2:B11)</f>
         <v>600</v>
@@ -5120,17 +5144,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.73046875" customWidth="1"/>
-    <col min="2" max="8" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="8" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -5165,7 +5189,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5203,7 +5227,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5241,7 +5265,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5279,7 +5303,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5317,7 +5341,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5355,7 +5379,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5393,7 +5417,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5431,7 +5455,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5469,7 +5493,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5507,7 +5531,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>

</xml_diff>